<commit_message>
Scripts Modificados - Detalle de trab
Mariela
</commit_message>
<xml_diff>
--- a/Documentacion - Diagramas/Detalle proyecto.xlsx
+++ b/Documentacion - Diagramas/Detalle proyecto.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -18,12 +18,76 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+  <si>
+    <t>Datos de llenado</t>
+  </si>
+  <si>
+    <t>https://mockaroo.com/</t>
+  </si>
+  <si>
+    <t>9:30-12md</t>
+  </si>
+  <si>
+    <t>Mariela</t>
+  </si>
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ESTUDIANTE</t>
+  </si>
+  <si>
+    <t>HORARIO</t>
+  </si>
+  <si>
+    <t>HRS TRAB</t>
+  </si>
+  <si>
+    <t>DETALLE</t>
+  </si>
+  <si>
+    <t>MariPaz</t>
+  </si>
+  <si>
+    <t>15/3/2018</t>
+  </si>
+  <si>
+    <t>16/3/2018</t>
+  </si>
+  <si>
+    <t>8-11pm</t>
+  </si>
+  <si>
+    <t>Creacion de bitacora en Github</t>
+  </si>
+  <si>
+    <t>Scripts de creacion de tablas</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +110,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -331,12 +407,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>